<commit_message>
complete pmi and working on nmi data
</commit_message>
<xml_diff>
--- a/nmi/comments.xlsx
+++ b/nmi/comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanjz\Desktop\python\nmi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B63B453F-0358-4FF1-B6EC-2B22F4662209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91AD325-01FD-4C6F-A104-730FFC6070F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3157" yWindow="3157" windowWidth="21601" windowHeight="11333" xr2:uid="{08871C9B-660B-4E47-80F7-171E63CDC1E3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{08871C9B-660B-4E47-80F7-171E63CDC1E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Industry</t>
   </si>
   <si>
-    <t>WHAT RESPONDENTS ARE SAYING</t>
-  </si>
-  <si>
     <t>Accommodation &amp; Food Services</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Utility contractors in high demand.</t>
+  </si>
+  <si>
+    <t>8/1/2023</t>
   </si>
 </sst>
 </file>
@@ -163,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,7 +222,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F1218BF-9F1E-41D1-ADA6-882763F52D51}" name="WHAT_RESPONDENTS_ARE_SAYING" displayName="WHAT_RESPONDENTS_ARE_SAYING" ref="A1:B11" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{EEAFC5F6-84F0-4EAD-A5E4-4074D8831FC2}" uniqueName="1" name="Industry" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{AD91E0F1-7835-4723-B53C-11281E737AB6}" uniqueName="2" name="WHAT RESPONDENTS ARE SAYING" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{AD91E0F1-7835-4723-B53C-11281E737AB6}" uniqueName="2" name="8/1/2023" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -546,100 +547,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BCAD83-26A2-475E-852B-3FF706C3D62D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>